<commit_message>
Update in submodule: LongGenBench_Test
</commit_message>
<xml_diff>
--- a/Evalution/preds_greedy/_cache_data.xlsx
+++ b/Evalution/preds_greedy/_cache_data.xlsx
@@ -8,6 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="qwen2.5" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="phi4" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -443,11 +444,11 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>preds_ns5_ws200_st20.0_ea1.0_snks0_hopf_True_type_snapkv_lenNone_gblFalse</t>
+          <t>preds_ns5_ws3_st20.0_ea1.0_snks0_hopf_False_type_max_fused_lenNone_gblFalse</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0</v>
+        <v>9591.93088</v>
       </c>
     </row>
     <row r="3">
@@ -467,7 +468,93 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>2469.246976</v>
+        <v>12283.930624</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>preds_ns5_ws200_st10.0_ea1.0_snks0_hopf_True_type_h2o_lenNone_gblFalse</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>17808.02688</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>preds_ns5_ws200_st20.0_ea1.0_snks0_hopf_True_type_snapkv_lenNone_gblFalse</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>phi4</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>preds_ns5_ws200_st20.0_ea1.0_snks0_hopf_True_type_sum_fused_lenNone_gblFalse</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>44093.696</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>preds_ns5_ws200_st10.0_ea1.0_snks0_hopf_True_type_h2o_lenNone_gblFalse</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>36342.912</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="1" t="inlineStr">
+        <is>
+          <t>preds_ns5_ws200_st20.0_ea1.0_snks0_hopf_True_type_max_fused_lenNone_gblFalse</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>44093.696</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>preds_ns5_ws32_st1025.0_ea1.0_snks0_hopf_True_type_snapkv_lenNone_gblFalse</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>140582.0928</v>
       </c>
     </row>
   </sheetData>

</xml_diff>